<commit_message>
Ejercicios y comentarios agregados
</commit_message>
<xml_diff>
--- a/Metodo Segundo Parcial/Metodo Polinomial Newton.xlsx
+++ b/Metodo Segundo Parcial/Metodo Polinomial Newton.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Analisis Numerico Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Analisis Numerico Git\Metodo Segundo Parcial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2D83FA-CE07-40BE-ADA2-ECA1EDC05EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA37F1BA-055F-4FFF-8022-9FE128C27A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{11656582-87E7-403F-B128-49AC355BCE63}"/>
+    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" firstSheet="2" activeTab="3" xr2:uid="{11656582-87E7-403F-B128-49AC355BCE63}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Polinomio De Netwon" sheetId="1" r:id="rId1"/>
+    <sheet name="Ejercicio 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Ejercicio 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Ejercicio 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>Metodo de Interpolacion Polinomial De Newton</t>
   </si>
@@ -52,6 +55,153 @@
   </si>
   <si>
     <t>//Con Symbolab</t>
+  </si>
+  <si>
+    <t>Se escribe con Coma en symbo</t>
+  </si>
+  <si>
+    <t>Rta:</t>
+  </si>
+  <si>
+    <t>0.8456x^3-1.0604x^2+1.933x+1</t>
+  </si>
+  <si>
+    <t>Si hay 6 n, entonces tiene que haber 5 terminos ademas del independiente</t>
+  </si>
+  <si>
+    <t>Independiente</t>
+  </si>
+  <si>
+    <t>*(x-1)</t>
+  </si>
+  <si>
+    <t>primer termino</t>
+  </si>
+  <si>
+    <t>*(x-0)</t>
+  </si>
+  <si>
+    <t>Segundo</t>
+  </si>
+  <si>
+    <t>Tercero</t>
+  </si>
+  <si>
+    <t>cuarto</t>
+  </si>
+  <si>
+    <t>*(x-0.5)</t>
+  </si>
+  <si>
+    <t>quinto</t>
+  </si>
+  <si>
+    <t>*(x-0.5)*(x-1)*(x-1.5)*(x-2)*(x-2.5)</t>
+  </si>
+  <si>
+    <t>(x-x0)</t>
+  </si>
+  <si>
+    <t>(x-x1)</t>
+  </si>
+  <si>
+    <t>(x-x3)</t>
+  </si>
+  <si>
+    <t>(x-x4)</t>
+  </si>
+  <si>
+    <t>(x-x2)</t>
+  </si>
+  <si>
+    <t>*(x-0.5)*(x-1)</t>
+  </si>
+  <si>
+    <t>*(x-0.5)*(x-1)*(x-1,5)</t>
+  </si>
+  <si>
+    <t>*(x-0.5)*(x-1)*(x-1,5)*(x-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTA: </t>
+  </si>
+  <si>
+    <t>0.01x^5-0.125x^4+1.2251x^3-3.66255x^2+5.8029x-1.13145</t>
+  </si>
+  <si>
+    <t>Excelente Resultado</t>
+  </si>
+  <si>
+    <t>Modelo para xi=0 hasta xi=6</t>
+  </si>
+  <si>
+    <t>Modelo para xi=0 hasta xi=5</t>
+  </si>
+  <si>
+    <t>*(x-1)*(x-2)</t>
+  </si>
+  <si>
+    <t>*(x-1)*(x-2)*(x-3)</t>
+  </si>
+  <si>
+    <t>*(x-1)*(x-2)*(x-3)*(x-5)</t>
+  </si>
+  <si>
+    <t>Si hay 5 n, entonces tiene que haber 4 terminos ademas del independiente</t>
+  </si>
+  <si>
+    <t>LOS NUMEROS QUE ACOMPAÑAN A X HAY QUE CAMBIARLOS DEPENDIENDO LAS X DE DATOS!!!!</t>
+  </si>
+  <si>
+    <t>NO OLVIDAR!!!</t>
+  </si>
+  <si>
+    <t>0.25x^3-0.5x^2-x+5.5</t>
+  </si>
+  <si>
+    <t>Si hay 7 n, entonces tiene que haber 6 terminos ademas del independiente</t>
+  </si>
+  <si>
+    <t>sexto</t>
+  </si>
+  <si>
+    <t>*(x-0)*(x-10)*(x-20)*(x-30)*(x-40)*(x-50)</t>
+  </si>
+  <si>
+    <t>*(x-0)*(x-10)</t>
+  </si>
+  <si>
+    <t>*(x-0)*(x-10)*(x-20)</t>
+  </si>
+  <si>
+    <t>*(x-0)*(x-10)*(x-20)*(x-30)</t>
+  </si>
+  <si>
+    <t>*(x-0)*(x-10)*(x-20)*(x-30)*(x-40)</t>
+  </si>
+  <si>
+    <t>(x-x5)</t>
+  </si>
+  <si>
+    <t>Modelo para xi=0 hasta xi=7</t>
+  </si>
+  <si>
+    <t>50000-1500*(x-0)+55*(x-0)*(x-10)-3*(x-0)*(x-10)*(x-20)+0.145833*(x-0)*(x-10)*(x-20)*(x-30)-0.0056666*(x-0)*(x-10)*(x-20)*(x-30)*(x-40)+0.000179*(x-0)*(x-10)*(x-20)*(x-30)*(x-40)*(x-50)</t>
+  </si>
+  <si>
+    <t>0.000179x^6-0.0325166x^5+2.233993x^4-71.85808x^3+1079.2063x^2-7032.982x+50000</t>
+  </si>
+  <si>
+    <t>Lo uso para copiar en Symbo:</t>
+  </si>
+  <si>
+    <t>Con puntos</t>
+  </si>
+  <si>
+    <t>1+1.7182*(x-0)+1.47635*(x-0)*(x-1)+0.8454666*(x-0)*(x-1)*(x-2)</t>
+  </si>
+  <si>
+    <t>0.8454666x^3-1.0600498x^2+1.9327832x+1</t>
   </si>
 </sst>
 </file>
@@ -75,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +241,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDC3939"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -187,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,6 +409,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB111CB-411D-4121-9732-E1ECA6A0168B}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +798,9 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="15" t="s">
+        <v>56</v>
+      </c>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -744,27 +947,16 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1">
-        <f>M2</f>
-        <v>1</v>
-      </c>
-      <c r="M7" s="1" t="str">
-        <f>"+"&amp;M3&amp;"*x"</f>
-        <v>+1,7182*x</v>
-      </c>
-      <c r="N7" s="1" t="str">
-        <f>"+("&amp;M3*(C5*-1)&amp;")"</f>
-        <v>+(0)</v>
-      </c>
-      <c r="O7" s="1" t="str">
-        <f>"+"&amp;M4&amp;"*x"</f>
-        <v>+1,47635*x</v>
-      </c>
-      <c r="P7" s="1" t="str">
-        <f>"+("&amp;M4*C5&amp;")"</f>
-        <v>+(0)</v>
-      </c>
+      <c r="K7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
@@ -840,7 +1032,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="K11" s="1"/>
@@ -861,7 +1053,9 @@
       <c r="G12" s="8"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1026,4 +1220,1680 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E646695-A952-4F0A-95CF-78DFE98C2DD0}">
+  <dimension ref="A2:O32"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <f>(C6-C5)/(B6-B5)</f>
+        <v>2.2380000000000004</v>
+      </c>
+      <c r="E5" s="3">
+        <f>(D6-D5)/(B7-B5)</f>
+        <v>-0.65600000000000058</v>
+      </c>
+      <c r="F5" s="3">
+        <f>(E6-E5)/(B8-B5)</f>
+        <v>0.76266666666666671</v>
+      </c>
+      <c r="G5" s="2">
+        <f>(F6-F5)/(B9-B5)</f>
+        <v>-5.0666666666666416E-2</v>
+      </c>
+      <c r="H5" s="3">
+        <f>(G6-G5)/(B10-B5)</f>
+        <v>1.0666666666666557E-2</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.1190000000000002</v>
+      </c>
+      <c r="D6" s="3">
+        <f>(C7-C6)/(B7-B6)</f>
+        <v>1.5819999999999999</v>
+      </c>
+      <c r="E6" s="3">
+        <f>(D7-D6)/(B8-B6)</f>
+        <v>0.48799999999999955</v>
+      </c>
+      <c r="F6" s="3">
+        <f>(E7-E6)/(B9-B6)</f>
+        <v>0.66133333333333388</v>
+      </c>
+      <c r="G6" s="2">
+        <f>(F7-F6)/(B10-B6)</f>
+        <v>-2.4000000000000021E-2</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2.91</v>
+      </c>
+      <c r="D7" s="3">
+        <f>(C8-C7)/(B8-B7)</f>
+        <v>2.0699999999999994</v>
+      </c>
+      <c r="E7" s="3">
+        <f>(D8-D7)/(B9-B7)</f>
+        <v>1.4800000000000004</v>
+      </c>
+      <c r="F7" s="3">
+        <f>(E8-E7)/(B10-B7)</f>
+        <v>0.61333333333333384</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3.9449999999999998</v>
+      </c>
+      <c r="D8" s="3">
+        <f>(C9-C8)/(B9-B8)</f>
+        <v>3.55</v>
+      </c>
+      <c r="E8" s="3">
+        <f>(D9-D8)/(B10-B8)</f>
+        <v>2.4000000000000012</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5.72</v>
+      </c>
+      <c r="D9" s="3">
+        <f>(C10-C9)/(B10-B9)</f>
+        <v>5.9500000000000011</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8.6950000000000003</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2">
+        <f>C5</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
+        <f>D5</f>
+        <v>2.2380000000000004</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2">
+        <f>E5</f>
+        <v>-0.65600000000000058</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2">
+        <f>F5</f>
+        <v>0.76266666666666671</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2">
+        <f>G5</f>
+        <v>-5.0666666666666416E-2</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3">
+        <f>H5</f>
+        <v>1.0666666666666557E-2</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E9CECC-DBE9-4646-9893-2D465F530E46}">
+  <dimension ref="A2:O32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="D5" s="3">
+        <f>(C6-C5)/(B6-B5)</f>
+        <v>-0.75</v>
+      </c>
+      <c r="E5" s="3">
+        <f>(D6-D5)/(B7-B5)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <f>(E6-E5)/(B8-B5)</f>
+        <v>0.25</v>
+      </c>
+      <c r="G5" s="2">
+        <f>(F6-F5)/(B9-B5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3">
+        <f>(C7-C6)/(B7-B6)</f>
+        <v>1.25</v>
+      </c>
+      <c r="E6" s="3">
+        <f>(D7-D6)/(B8-B6)</f>
+        <v>2</v>
+      </c>
+      <c r="F6" s="3">
+        <f>(E7-E6)/(B9-B6)</f>
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>5.25</v>
+      </c>
+      <c r="D7" s="3">
+        <f>(C8-C7)/(B8-B7)</f>
+        <v>7.25</v>
+      </c>
+      <c r="E7" s="3">
+        <f>(D8-D7)/(B9-B7)</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>19.75</v>
+      </c>
+      <c r="D8" s="3">
+        <f>(C9-C8)/(B9-B8)</f>
+        <v>16.25</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2">
+        <f>C5</f>
+        <v>4.75</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
+        <f>D5</f>
+        <v>-0.75</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="J25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2">
+        <f>E5</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2">
+        <f>F5</f>
+        <v>0.25</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2">
+        <f>G5</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93DA6945-95A6-4E94-8C67-6B91E1AE1703}">
+  <dimension ref="A2:Z34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="20"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>50000</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D10" si="0">(C6-C5)/(B6-B5)</f>
+        <v>-1500</v>
+      </c>
+      <c r="E5" s="3">
+        <f>(D6-D5)/(B7-B5)</f>
+        <v>55</v>
+      </c>
+      <c r="F5" s="3">
+        <f>(E6-E5)/(B8-B5)</f>
+        <v>-3</v>
+      </c>
+      <c r="G5" s="2">
+        <f>(F6-F5)/(B9-B5)</f>
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="H5" s="3">
+        <f>(G6-G5)/(B10-B5)</f>
+        <v>-5.6666666666666662E-3</v>
+      </c>
+      <c r="I5" s="3">
+        <f>(H6-H5)/(B11-B5)</f>
+        <v>1.7916666666666664E-4</v>
+      </c>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>35000</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>-400</v>
+      </c>
+      <c r="E6" s="3">
+        <f>(D7-D6)/(B8-B6)</f>
+        <v>-35</v>
+      </c>
+      <c r="F6" s="3">
+        <f>(E7-E6)/(B9-B6)</f>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="G6" s="2">
+        <f>(F7-F6)/(B10-B6)</f>
+        <v>-0.13750000000000001</v>
+      </c>
+      <c r="H6" s="3">
+        <f>(G7-G6)/(B11-B6)</f>
+        <v>5.0833333333333329E-3</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>31000</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>-1100</v>
+      </c>
+      <c r="E7" s="3">
+        <f>(D8-D7)/(B9-B7)</f>
+        <v>50</v>
+      </c>
+      <c r="F7" s="3">
+        <f>(E8-E7)/(B10-B7)</f>
+        <v>-2.6666666666666665</v>
+      </c>
+      <c r="G7" s="2">
+        <f>(F8-F7)/(B11-B7)</f>
+        <v>0.11666666666666665</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3">
+        <v>20000</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E8" s="3">
+        <f>(D9-D8)/(B10-B8)</f>
+        <v>-30</v>
+      </c>
+      <c r="F8" s="3">
+        <f>(E9-E8)/(B11-B8)</f>
+        <v>2</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3">
+        <v>19000</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>-700</v>
+      </c>
+      <c r="E9" s="3">
+        <f>(D10-D9)/(B11-B9)</f>
+        <v>30</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3">
+        <v>12000</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>60</v>
+      </c>
+      <c r="C11" s="3">
+        <v>11000</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2">
+        <f>C5</f>
+        <v>50000</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
+        <f>D5</f>
+        <v>-1500</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="J25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2">
+        <f>E5</f>
+        <v>55</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2">
+        <f>F5</f>
+        <v>-3</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2">
+        <f>G5</f>
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3">
+        <f>H5</f>
+        <v>-5.6666666666666662E-3</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="K29" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2">
+        <f>I5</f>
+        <v>1.7916666666666664E-4</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="23"/>
+      <c r="W30" s="23"/>
+      <c r="X30" s="23"/>
+      <c r="Y30" s="23"/>
+      <c r="Z30" s="23"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cosas subidas del todo
</commit_message>
<xml_diff>
--- a/Metodo Segundo Parcial/Metodo Polinomial Newton.xlsx
+++ b/Metodo Segundo Parcial/Metodo Polinomial Newton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Analisis Numerico Git\Metodo Segundo Parcial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA37F1BA-055F-4FFF-8022-9FE128C27A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2704C08A-AF44-42B9-891F-15E5728E9CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" firstSheet="2" activeTab="3" xr2:uid="{11656582-87E7-403F-B128-49AC355BCE63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{11656582-87E7-403F-B128-49AC355BCE63}"/>
   </bookViews>
   <sheets>
     <sheet name="Polinomio De Netwon" sheetId="1" r:id="rId1"/>
@@ -445,6 +445,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D408587B-93B2-865C-AF69-93CC88A8AF35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12220575" y="581025"/>
+          <a:ext cx="5067300" cy="4448175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -746,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB111CB-411D-4121-9732-E1ECA6A0168B}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +924,6 @@
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -927,7 +992,6 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1081,7 +1145,6 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1219,6 +1282,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2279,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93DA6945-95A6-4E94-8C67-6B91E1AE1703}">
   <dimension ref="A2:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>